<commit_message>
uz vypisuje excel po listech
</commit_message>
<xml_diff>
--- a/test_assets/dochazka-duben.xlsx
+++ b/test_assets/dochazka-duben.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="List2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="List1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="List2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="14">
   <si>
     <t xml:space="preserve">Jméno</t>
   </si>
@@ -40,7 +41,7 @@
     <t xml:space="preserve">Odchod</t>
   </si>
   <si>
-    <t xml:space="preserve">Adam</t>
+    <t xml:space="preserve">Pavel</t>
   </si>
   <si>
     <t xml:space="preserve">Sucharda</t>
@@ -52,13 +53,16 @@
     <t xml:space="preserve">P</t>
   </si>
   <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
     <t xml:space="preserve">SC</t>
   </si>
   <si>
-    <t xml:space="preserve">D</t>
+    <t xml:space="preserve">SV</t>
   </si>
   <si>
-    <t xml:space="preserve">SV</t>
+    <t xml:space="preserve">Adam</t>
   </si>
 </sst>
 </file>
@@ -182,10 +186,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -230,13 +234,9 @@
       <c r="F2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <f aca="false">F2-E2</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -255,13 +255,9 @@
       <c r="F3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <f aca="false">F3-E3</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -280,13 +276,9 @@
       <c r="F4" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <f aca="false">F4-E4</f>
-        <v>2</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -305,16 +297,9 @@
       <c r="F5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <f aca="false">F5-E5</f>
-        <v>14</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -325,7 +310,7 @@
         <v>45021</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>0</v>
@@ -333,13 +318,9 @@
       <c r="F6" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <f aca="false">F6-E6</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -358,16 +339,9 @@
       <c r="F7" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <f aca="false">F7-E7</f>
-        <v>8</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -386,16 +360,9 @@
       <c r="F8" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <f aca="false">F8-E8</f>
-        <v>8</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -414,13 +381,9 @@
       <c r="F9" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="0" t="n">
-        <f aca="false">F9-E9</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -431,21 +394,17 @@
         <v>45025</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <f aca="false">F10-E10</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -464,16 +423,9 @@
       <c r="F11" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G11" s="0" t="n">
-        <f aca="false">F11-E11</f>
-        <v>8</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -492,13 +444,9 @@
       <c r="F12" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G12" s="0" t="n">
-        <f aca="false">F12-E12</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -517,13 +465,9 @@
       <c r="F13" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="0" t="n">
-        <f aca="false">F13-E13</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -542,16 +486,9 @@
       <c r="F14" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G14" s="0" t="n">
-        <f aca="false">F14-E14</f>
-        <v>8</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -570,16 +507,9 @@
       <c r="F15" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <f aca="false">F15-E15</f>
-        <v>8</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -598,13 +528,9 @@
       <c r="F16" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="0" t="n">
-        <f aca="false">F16-E16</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -623,13 +549,9 @@
       <c r="F17" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="0" t="n">
-        <f aca="false">F17-E17</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -648,16 +570,9 @@
       <c r="F18" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G18" s="0" t="n">
-        <f aca="false">F18-E18</f>
-        <v>8</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -668,7 +583,7 @@
         <v>45034</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E19" s="3" t="n">
         <v>8</v>
@@ -676,16 +591,9 @@
       <c r="F19" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G19" s="0" t="n">
-        <f aca="false">F19-E19</f>
-        <v>8</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -696,24 +604,17 @@
         <v>45035</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" s="3" t="n">
         <v>8</v>
       </c>
       <c r="F20" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <f aca="false">F20-E20</f>
-        <v>8</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -724,7 +625,7 @@
         <v>45036</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E21" s="3" t="n">
         <v>8</v>
@@ -732,16 +633,9 @@
       <c r="F21" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G21" s="0" t="n">
-        <f aca="false">F21-E21</f>
-        <v>8</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -760,16 +654,9 @@
       <c r="F22" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G22" s="0" t="n">
-        <f aca="false">F22-E22</f>
-        <v>8</v>
-      </c>
-      <c r="H22" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -788,13 +675,9 @@
       <c r="F23" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G23" s="0" t="n">
-        <f aca="false">F23-E23</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -813,13 +696,9 @@
       <c r="F24" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G24" s="0" t="n">
-        <f aca="false">F24-E24</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -838,16 +717,9 @@
       <c r="F25" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G25" s="0" t="n">
-        <f aca="false">F25-E25</f>
-        <v>8</v>
-      </c>
-      <c r="H25" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -866,16 +738,9 @@
       <c r="F26" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G26" s="0" t="n">
-        <f aca="false">F26-E26</f>
-        <v>8</v>
-      </c>
-      <c r="H26" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -894,16 +759,9 @@
       <c r="F27" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G27" s="0" t="n">
-        <f aca="false">F27-E27</f>
-        <v>8</v>
-      </c>
-      <c r="H27" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -922,16 +780,9 @@
       <c r="F28" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G28" s="0" t="n">
-        <f aca="false">F28-E28</f>
-        <v>8</v>
-      </c>
-      <c r="H28" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -950,16 +801,9 @@
       <c r="F29" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G29" s="0" t="n">
-        <f aca="false">F29-E29</f>
-        <v>8</v>
-      </c>
-      <c r="H29" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -978,13 +822,9 @@
       <c r="F30" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="0" t="n">
-        <f aca="false">F30-E30</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -1003,23 +843,683 @@
       <c r="F31" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="0" t="n">
-        <f aca="false">F31-E31</f>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <f aca="false">DATE(2023,4,1)</f>
+        <v>45017</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <f aca="false">C2+1</f>
+        <v>45018</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <f aca="false">C3+1</f>
+        <v>45019</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <f aca="false">C4+1</f>
+        <v>45020</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <f aca="false">C5+1</f>
+        <v>45021</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <f aca="false">C6+1</f>
+        <v>45022</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <f aca="false">C7+1</f>
+        <v>45023</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <f aca="false">C8+1</f>
+        <v>45024</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <f aca="false">C9+1</f>
+        <v>45025</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <f aca="false">C10+1</f>
+        <v>45026</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <f aca="false">C11+1</f>
+        <v>45027</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <f aca="false">C12+1</f>
+        <v>45028</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <f aca="false">C13+1</f>
+        <v>45029</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <f aca="false">C14+1</f>
+        <v>45030</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <f aca="false">C15+1</f>
+        <v>45031</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <f aca="false">C16+1</f>
+        <v>45032</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <f aca="false">C17+1</f>
+        <v>45033</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <f aca="false">C18+1</f>
+        <v>45034</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <f aca="false">C19+1</f>
+        <v>45035</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <f aca="false">C20+1</f>
+        <v>45036</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <f aca="false">C21+1</f>
+        <v>45037</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <f aca="false">C22+1</f>
+        <v>45038</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <f aca="false">C23+1</f>
+        <v>45039</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <f aca="false">C24+1</f>
+        <v>45040</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <f aca="false">C25+1</f>
+        <v>45041</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <f aca="false">C26+1</f>
+        <v>45042</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <f aca="false">C27+1</f>
+        <v>45043</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <f aca="false">C28+1</f>
+        <v>45044</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <f aca="false">C29+1</f>
+        <v>45045</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <f aca="false">C30+1</f>
+        <v>45046</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="2"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="0" t="n">
-        <f aca="false">SUM(G$2:G$31)</f>
-        <v>136</v>
-      </c>
-      <c r="H32" s="0" t="n">
-        <f aca="false">SUM(H$2:H$31)</f>
-        <v>16</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
uprava vzorce pro vypocet stravneho za sluzebni cesty
</commit_message>
<xml_diff>
--- a/test_assets/dochazka-duben.xlsx
+++ b/test_assets/dochazka-duben.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="14">
   <si>
     <t xml:space="preserve">Jméno</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t xml:space="preserve">Odchod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Km</t>
   </si>
   <si>
     <t xml:space="preserve">Pavel</t>
@@ -197,10 +194,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -224,23 +221,21 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="n">
         <f aca="false">DATE(2023,4,1)</f>
         <v>45017</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>0</v>
@@ -251,17 +246,17 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="n">
         <f aca="false">C2+1</f>
         <v>45018</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>0</v>
@@ -272,17 +267,17 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4" t="n">
         <f aca="false">C3+1</f>
         <v>45019</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>8</v>
@@ -293,17 +288,17 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4" t="n">
         <f aca="false">C4+1</f>
         <v>45020</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>6</v>
@@ -314,17 +309,17 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="n">
         <f aca="false">C5+1</f>
         <v>45021</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="5" t="n">
         <v>0</v>
@@ -335,17 +330,17 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4" t="n">
         <f aca="false">C6+1</f>
         <v>45022</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>8</v>
@@ -356,17 +351,17 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="4" t="n">
         <f aca="false">C7+1</f>
         <v>45023</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="5" t="n">
         <v>8</v>
@@ -377,17 +372,17 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4" t="n">
         <f aca="false">C8+1</f>
         <v>45024</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>0</v>
@@ -398,41 +393,38 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="4" t="n">
         <f aca="false">C9+1</f>
         <v>45025</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>8</v>
       </c>
       <c r="F10" s="5" t="n">
         <v>16</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>150</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="4" t="n">
         <f aca="false">C10+1</f>
         <v>45026</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>8</v>
@@ -443,17 +435,17 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="4" t="n">
         <f aca="false">C11+1</f>
         <v>45027</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>0</v>
@@ -464,17 +456,17 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="4" t="n">
         <f aca="false">C12+1</f>
         <v>45028</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>0</v>
@@ -485,17 +477,17 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="4" t="n">
         <f aca="false">C13+1</f>
         <v>45029</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>8</v>
@@ -506,17 +498,17 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="4" t="n">
         <f aca="false">C14+1</f>
         <v>45030</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>8</v>
@@ -527,17 +519,17 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="4" t="n">
         <f aca="false">C15+1</f>
         <v>45031</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>0</v>
@@ -548,17 +540,17 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="4" t="n">
         <f aca="false">C16+1</f>
         <v>45032</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>0</v>
@@ -569,17 +561,17 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="4" t="n">
         <f aca="false">C17+1</f>
         <v>45033</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>8</v>
@@ -590,41 +582,38 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="4" t="n">
         <f aca="false">C18+1</f>
         <v>45034</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>8</v>
       </c>
       <c r="F19" s="5" t="n">
         <v>16</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>58</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="4" t="n">
         <f aca="false">C19+1</f>
         <v>45035</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>8</v>
@@ -635,41 +624,38 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" s="4" t="n">
         <f aca="false">C20+1</f>
         <v>45036</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>8</v>
       </c>
       <c r="F21" s="5" t="n">
         <v>16</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <v>64</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="4" t="n">
         <f aca="false">C21+1</f>
         <v>45037</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>8</v>
@@ -680,17 +666,17 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" s="4" t="n">
         <f aca="false">C22+1</f>
         <v>45038</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>0</v>
@@ -701,17 +687,17 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="4" t="n">
         <f aca="false">C23+1</f>
         <v>45039</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>0</v>
@@ -722,17 +708,17 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" s="4" t="n">
         <f aca="false">C24+1</f>
         <v>45040</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>8</v>
@@ -743,17 +729,17 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" s="4" t="n">
         <f aca="false">C25+1</f>
         <v>45041</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>8</v>
@@ -764,17 +750,17 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="4" t="n">
         <f aca="false">C26+1</f>
         <v>45042</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>8</v>
@@ -785,17 +771,17 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" s="4" t="n">
         <f aca="false">C27+1</f>
         <v>45043</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>8</v>
@@ -806,17 +792,17 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" s="4" t="n">
         <f aca="false">C28+1</f>
         <v>45044</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>8</v>
@@ -827,17 +813,17 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" s="4" t="n">
         <f aca="false">C29+1</f>
         <v>45045</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>0</v>
@@ -848,29 +834,23 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31" s="4" t="n">
         <f aca="false">C30+1</f>
         <v>45046</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F31" s="5" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G32" s="0" t="n">
-        <f aca="false">SUM(G$2:G$31)</f>
-        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -889,10 +869,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -916,23 +896,21 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="n">
         <f aca="false">DATE(2023,4,1)</f>
         <v>45017</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>0</v>
@@ -943,17 +921,17 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="n">
         <f aca="false">C2+1</f>
         <v>45018</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>0</v>
@@ -964,17 +942,17 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4" t="n">
         <f aca="false">C3+1</f>
         <v>45019</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>8</v>
@@ -985,17 +963,17 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4" t="n">
         <f aca="false">C4+1</f>
         <v>45020</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>6</v>
@@ -1003,23 +981,20 @@
       <c r="F5" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>250</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="n">
         <f aca="false">C5+1</f>
         <v>45021</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="5" t="n">
         <v>0</v>
@@ -1030,17 +1005,17 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4" t="n">
         <f aca="false">C6+1</f>
         <v>45022</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>8</v>
@@ -1052,17 +1027,17 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="4" t="n">
         <f aca="false">C7+1</f>
         <v>45023</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="5" t="n">
         <v>8</v>
@@ -1074,17 +1049,17 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4" t="n">
         <f aca="false">C8+1</f>
         <v>45024</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>0</v>
@@ -1095,17 +1070,17 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="4" t="n">
         <f aca="false">C9+1</f>
         <v>45025</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>0</v>
@@ -1116,17 +1091,17 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="4" t="n">
         <f aca="false">C10+1</f>
         <v>45026</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>8</v>
@@ -1138,17 +1113,17 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="4" t="n">
         <f aca="false">C11+1</f>
         <v>45027</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>0</v>
@@ -1159,17 +1134,17 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="4" t="n">
         <f aca="false">C12+1</f>
         <v>45028</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>0</v>
@@ -1180,17 +1155,17 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="4" t="n">
         <f aca="false">C13+1</f>
         <v>45029</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>8</v>
@@ -1202,17 +1177,17 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="4" t="n">
         <f aca="false">C14+1</f>
         <v>45030</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>8</v>
@@ -1224,17 +1199,17 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="4" t="n">
         <f aca="false">C15+1</f>
         <v>45031</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>0</v>
@@ -1245,17 +1220,17 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="4" t="n">
         <f aca="false">C16+1</f>
         <v>45032</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>0</v>
@@ -1266,17 +1241,17 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="4" t="n">
         <f aca="false">C17+1</f>
         <v>45033</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>8</v>
@@ -1288,89 +1263,80 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="4" t="n">
         <f aca="false">C18+1</f>
         <v>45034</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>8</v>
       </c>
       <c r="F19" s="5" t="n">
         <v>16</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>150</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="4" t="n">
         <f aca="false">C19+1</f>
         <v>45035</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>8</v>
       </c>
       <c r="F20" s="5" t="n">
         <v>16</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" s="4" t="n">
         <f aca="false">C20+1</f>
         <v>45036</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>8</v>
       </c>
       <c r="F21" s="5" t="n">
         <v>16</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <v>250</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="4" t="n">
         <f aca="false">C21+1</f>
         <v>45037</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>8</v>
@@ -1382,17 +1348,17 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" s="4" t="n">
         <f aca="false">C22+1</f>
         <v>45038</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>0</v>
@@ -1403,17 +1369,17 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="4" t="n">
         <f aca="false">C23+1</f>
         <v>45039</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>0</v>
@@ -1424,17 +1390,17 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" s="4" t="n">
         <f aca="false">C24+1</f>
         <v>45040</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>8</v>
@@ -1446,17 +1412,17 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" s="4" t="n">
         <f aca="false">C25+1</f>
         <v>45041</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>8</v>
@@ -1468,17 +1434,17 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="4" t="n">
         <f aca="false">C26+1</f>
         <v>45042</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>8</v>
@@ -1490,17 +1456,17 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" s="4" t="n">
         <f aca="false">C27+1</f>
         <v>45043</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>8</v>
@@ -1512,17 +1478,17 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" s="4" t="n">
         <f aca="false">C28+1</f>
         <v>45044</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>8</v>
@@ -1534,17 +1500,17 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" s="4" t="n">
         <f aca="false">C29+1</f>
         <v>45045</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>0</v>
@@ -1555,30 +1521,23 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31" s="4" t="n">
         <f aca="false">C30+1</f>
         <v>45046</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F31" s="5" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="4"/>
-      <c r="G32" s="6" t="n">
-        <f aca="false">SUM(G$2:G$31)</f>
-        <v>680</v>
       </c>
     </row>
   </sheetData>

</xml_diff>